<commit_message>
AutoCommit_1 ноября 2023 г. 10:13:33_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>2ИСИП-422: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -112,6 +112,27 @@
   </si>
   <si>
     <t>ОК</t>
+  </si>
+  <si>
+    <t>ДЗ1</t>
+  </si>
+  <si>
+    <t>ДЗ2</t>
+  </si>
+  <si>
+    <t>ДЗ3</t>
+  </si>
+  <si>
+    <t>ДЗ4</t>
+  </si>
+  <si>
+    <t>ДЗ5</t>
+  </si>
+  <si>
+    <t>ДЗ6</t>
+  </si>
+  <si>
+    <t>ДЗ7</t>
   </si>
 </sst>
 </file>
@@ -500,7 +521,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -535,21 +556,31 @@
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
     </row>
-    <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -620,14 +651,20 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -726,8 +763,11 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -741,7 +781,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -754,8 +794,11 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -769,7 +812,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -783,7 +826,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -797,7 +840,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -811,7 +854,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -825,7 +868,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -839,7 +882,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -853,7 +896,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -867,7 +910,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -881,7 +924,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -895,7 +938,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -909,7 +952,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -923,7 +966,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -937,7 +980,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_2 ноября 2023 г. 10:06:18_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>2ИСИП-422: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -518,10 +518,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -833,9 +833,15 @@
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_2 ноября 2023 г. 10:07:57_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>2ИСИП-422: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -521,7 +521,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -805,7 +805,9 @@
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_2 ноября 2023 г. 10:35:04_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>2ИСИП-422: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>ДЗ7</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -602,7 +605,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -616,21 +619,32 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -701,8 +715,12 @@
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -736,7 +754,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -750,24 +768,36 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -848,7 +878,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -862,21 +892,34 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -890,21 +933,36 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="C25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_8 ноября 2023 г. 10:08:06_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
     <t>2ИСИП-422: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>ок</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -197,11 +200,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -214,6 +228,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -521,10 +538,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -668,7 +685,9 @@
       <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>30</v>
       </c>
@@ -678,6 +697,9 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_8 ноября 2023 г. 10:41:36_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="40">
   <si>
     <t>2ИСИП-422: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -226,11 +226,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -538,10 +538,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -552,29 +552,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -698,7 +698,7 @@
       <c r="H9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -748,7 +748,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -762,19 +762,34 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -826,31 +841,58 @@
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -998,21 +1040,36 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -1026,7 +1083,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -1040,21 +1097,36 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1068,7 +1140,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -1082,21 +1154,36 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>

</xml_diff>

<commit_message>
AutoCommit_8 ноября 2023 г. 10:55:07_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="40">
   <si>
     <t>2ИСИП-422: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -538,10 +538,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18:I18"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,9 @@
       <c r="F9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="H9" s="2" t="s">
         <v>30</v>
       </c>
@@ -981,7 +983,9 @@
       <c r="H23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="2"/>
+      <c r="I23" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">

</xml_diff>

<commit_message>
AutoCommit_9 ноября 2023 г. 10:09:39_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="40">
   <si>
     <t>2ИСИП-422: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -538,10 +538,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -675,7 +675,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -704,21 +704,36 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -746,7 +761,9 @@
         <v>30</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
@@ -996,10 +1013,21 @@
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">

</xml_diff>

<commit_message>
AutoCommit_9 ноября 2023 г. 10:20:56_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
   <si>
     <t>2ИСИП-422: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -541,7 +541,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -927,7 +927,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -941,7 +941,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -957,9 +957,18 @@
       <c r="E21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">

</xml_diff>

<commit_message>
AutoCommit_9 ноября 2023 г. 13:39:08_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="40">
   <si>
     <t>2ИСИП-422: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -541,7 +541,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -629,12 +629,27 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -740,14 +755,29 @@
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -921,11 +951,24 @@
       <c r="C19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">

</xml_diff>

<commit_message>
AutoCommit_27 ноября 2023 г. 10:32:36_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -230,11 +230,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -542,10 +542,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -556,29 +556,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -708,15 +708,30 @@
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="4">
+        <v>5</v>
+      </c>
       <c r="K8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="M8">
         <v>2</v>
@@ -880,7 +895,7 @@
       <c r="H13" s="2">
         <v>5</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="6">
         <v>5</v>
       </c>
       <c r="K13" s="5">
@@ -1156,15 +1171,21 @@
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="C22" s="2">
+        <v>5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="K22" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M22">
         <v>2</v>
@@ -1213,8 +1234,12 @@
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
       <c r="E24" s="2">
         <v>5</v>
       </c>
@@ -1233,7 +1258,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="5">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M24">
         <v>4</v>
@@ -1282,15 +1307,30 @@
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="C26" s="2">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2">
+        <v>5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>5</v>
+      </c>
+      <c r="F26" s="2">
+        <v>5</v>
+      </c>
+      <c r="G26" s="2">
+        <v>5</v>
+      </c>
+      <c r="H26" s="2">
+        <v>5</v>
+      </c>
+      <c r="I26" s="6">
+        <v>5</v>
+      </c>
       <c r="K26" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="M26">
         <v>2</v>

</xml_diff>

<commit_message>
AutoCommit_27 ноября 2023 г. 10:33:10_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -542,10 +542,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1180,12 +1180,18 @@
       <c r="E22" s="2">
         <v>5</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
+      <c r="G22" s="2">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2">
+        <v>5</v>
+      </c>
       <c r="K22" s="5">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="M22">
         <v>2</v>

</xml_diff>

<commit_message>
AutoCommit_29 ноября 2023 г. 12:35:53_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -545,7 +545,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -949,15 +949,27 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2">
+        <v>5</v>
+      </c>
       <c r="K15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M15">
         <v>2</v>
@@ -1114,15 +1126,30 @@
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="C20" s="2">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2">
+        <v>5</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5</v>
+      </c>
+      <c r="I20" s="2">
+        <v>5</v>
+      </c>
       <c r="K20" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="M20">
         <v>2</v>

</xml_diff>

<commit_message>
AutoCommit_7 декабря 2023 г. 11:29:09_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -558,7 +558,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomRight" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -645,7 +645,7 @@
       </c>
       <c r="N4" s="9">
         <f t="shared" ref="N4:P4" si="0">SUM(N5:N33)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O4" s="9">
         <f t="shared" si="0"/>
@@ -1325,13 +1325,16 @@
         <v>5</v>
       </c>
       <c r="K19" s="5"/>
+      <c r="L19" s="8">
+        <v>2</v>
+      </c>
       <c r="M19" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N19" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" s="9">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
AutoCommit_7 декабря 2023 г. 11:41:57_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -558,7 +558,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L24" sqref="L24"/>
+      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1610,6 +1610,9 @@
       <c r="I25" s="2">
         <v>5</v>
       </c>
+      <c r="J25" s="4">
+        <v>5</v>
+      </c>
       <c r="K25" s="5"/>
       <c r="M25" s="9">
         <f t="shared" si="2"/>
@@ -1654,6 +1657,9 @@
         <v>5</v>
       </c>
       <c r="I26" s="6">
+        <v>5</v>
+      </c>
+      <c r="J26" s="6">
         <v>5</v>
       </c>
       <c r="K26" s="5"/>

</xml_diff>

<commit_message>
AutoCommit_7 декабря 2023 г. 13:18:29_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -555,10 +555,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -641,7 +641,7 @@
       <c r="H4" s="1"/>
       <c r="M4">
         <f>SUM(M5:M33)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N4" s="9">
         <f t="shared" ref="N4:P4" si="0">SUM(N5:N33)</f>
@@ -904,9 +904,12 @@
         <v>5</v>
       </c>
       <c r="K10" s="5"/>
+      <c r="L10" s="8">
+        <v>1</v>
+      </c>
       <c r="M10" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="9">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
AutoCommit_13 декабря 2023 г. 10:25:33_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -561,10 +561,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -675,12 +675,27 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
+      <c r="J5" s="6">
+        <v>5</v>
+      </c>
       <c r="L5">
         <v>1</v>
       </c>
@@ -866,7 +881,12 @@
       <c r="I9" s="4">
         <v>5</v>
       </c>
-      <c r="K9" s="5"/>
+      <c r="J9" s="4">
+        <v>5</v>
+      </c>
+      <c r="K9" s="4">
+        <v>5</v>
+      </c>
       <c r="L9" s="8">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_13 декабря 2023 г. 10:49:50_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -561,10 +561,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1879,7 +1879,12 @@
       <c r="I30" s="2">
         <v>5</v>
       </c>
-      <c r="K30" s="5"/>
+      <c r="J30" s="8">
+        <v>5</v>
+      </c>
+      <c r="K30" s="8">
+        <v>5</v>
+      </c>
       <c r="L30" s="8">
         <v>1</v>
       </c>
@@ -1993,7 +1998,12 @@
       <c r="I33" s="2">
         <v>5</v>
       </c>
-      <c r="K33" s="5"/>
+      <c r="J33" s="4">
+        <v>5</v>
+      </c>
+      <c r="K33" s="4">
+        <v>5</v>
+      </c>
       <c r="L33" s="8">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_13 декабря 2023 г. 18:49:27_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -561,10 +561,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
+      <selection pane="bottomRight" activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -693,6 +693,9 @@
       <c r="H5" s="2">
         <v>5</v>
       </c>
+      <c r="I5" s="4">
+        <v>5</v>
+      </c>
       <c r="J5" s="6">
         <v>5</v>
       </c>
@@ -1117,7 +1120,12 @@
       <c r="I14" s="2">
         <v>5</v>
       </c>
-      <c r="K14" s="5"/>
+      <c r="J14" s="4">
+        <v>5</v>
+      </c>
+      <c r="K14" s="4">
+        <v>5</v>
+      </c>
       <c r="L14" s="8">
         <v>2</v>
       </c>
@@ -1136,6 +1144,9 @@
       <c r="P14" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="R14">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1236,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -1264,7 +1275,12 @@
       <c r="I17" s="2">
         <v>5</v>
       </c>
-      <c r="K17" s="5"/>
+      <c r="J17" s="4">
+        <v>5</v>
+      </c>
+      <c r="K17" s="4">
+        <v>5</v>
+      </c>
       <c r="L17" s="8">
         <v>4</v>
       </c>
@@ -1285,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -1334,7 +1350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -1383,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -1429,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -1482,8 +1498,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1526,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -1575,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -1629,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -1680,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -1729,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -1783,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -1817,7 +1836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -1851,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1905,7 +1924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1939,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -1970,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -2023,8 +2042,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -2032,7 +2054,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="13" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_13 декабря 2023 г. 19:34:31_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -557,10 +557,10 @@
   <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="I20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="AB38" sqref="AB38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AutoCommit_14 декабря 2023 г. 11:34:10_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -557,10 +557,10 @@
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1240,6 +1240,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="S14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -1440,7 +1443,12 @@
       <c r="J18" s="2">
         <v>5</v>
       </c>
-      <c r="L18" s="5"/>
+      <c r="K18" s="6">
+        <v>5</v>
+      </c>
+      <c r="L18" s="8">
+        <v>5</v>
+      </c>
       <c r="M18" s="8">
         <v>2</v>
       </c>
@@ -2056,13 +2064,33 @@
       <c r="C30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="L30" s="5"/>
+      <c r="D30" s="2">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
+      <c r="F30" s="2">
+        <v>5</v>
+      </c>
+      <c r="G30" s="2">
+        <v>5</v>
+      </c>
+      <c r="H30" s="2">
+        <v>5</v>
+      </c>
+      <c r="I30" s="2">
+        <v>5</v>
+      </c>
+      <c r="J30" s="6">
+        <v>5</v>
+      </c>
+      <c r="K30" s="8">
+        <v>5</v>
+      </c>
+      <c r="L30" s="8">
+        <v>5</v>
+      </c>
       <c r="M30">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_15 декабря 2023 г. 14:09:56_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -169,7 +169,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +179,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -263,6 +269,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -572,10 +581,10 @@
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L37" sqref="L37"/>
+      <selection pane="bottomRight" activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1674,7 +1683,12 @@
       <c r="J22" s="10">
         <v>5</v>
       </c>
-      <c r="L22" s="4"/>
+      <c r="K22" s="14">
+        <v>5</v>
+      </c>
+      <c r="L22" s="14">
+        <v>5</v>
+      </c>
       <c r="M22" s="7">
         <v>1</v>
       </c>
@@ -1693,6 +1707,9 @@
       <c r="Q22" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="S22">
+        <v>5</v>
       </c>
       <c r="T22" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
AutoCommit_20 декабря 2023 г. 11:15:08_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -594,10 +594,10 @@
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -959,6 +959,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="S8">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -1053,7 +1056,12 @@
       <c r="J10" s="9">
         <v>5</v>
       </c>
-      <c r="L10" s="4"/>
+      <c r="K10" s="10">
+        <v>5</v>
+      </c>
+      <c r="L10" s="12">
+        <v>5</v>
+      </c>
       <c r="M10" s="16">
         <v>1</v>
       </c>
@@ -1150,14 +1158,21 @@
       <c r="G12" s="9">
         <v>5</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
       <c r="I12" s="9">
         <v>5</v>
       </c>
       <c r="J12" s="11">
         <v>5</v>
       </c>
-      <c r="L12" s="4"/>
+      <c r="K12" s="11">
+        <v>5</v>
+      </c>
+      <c r="L12" s="12">
+        <v>5</v>
+      </c>
       <c r="M12" s="14">
         <v>4</v>
       </c>
@@ -1177,6 +1192,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="S12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -1330,6 +1348,9 @@
         <v>5</v>
       </c>
       <c r="J15" s="9">
+        <v>5</v>
+      </c>
+      <c r="K15" s="11">
         <v>5</v>
       </c>
       <c r="L15" s="4"/>
@@ -1523,6 +1544,9 @@
       <c r="Q18" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="S18">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2176,6 +2200,9 @@
       <c r="Q30" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="S30">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_20 декабря 2023 г. 11:38:25_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -594,10 +594,10 @@
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -773,6 +773,9 @@
       <c r="J5" s="10">
         <v>5</v>
       </c>
+      <c r="K5" s="10">
+        <v>5</v>
+      </c>
       <c r="L5" s="4"/>
       <c r="N5" s="7">
         <f t="shared" si="1"/>
@@ -884,7 +887,12 @@
       <c r="J7" s="10">
         <v>5</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="K7" s="13">
+        <v>5</v>
+      </c>
+      <c r="L7" s="13">
+        <v>5</v>
+      </c>
       <c r="N7" s="7">
         <f t="shared" si="1"/>
         <v>0</v>

</xml_diff>

<commit_message>
AutoCommit_20 декабря 2023 г. 11:49:20_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -242,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -285,6 +285,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -597,14 +600,14 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomRight" activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
     <col min="2" max="2" width="25.36328125" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" customWidth="1"/>
+    <col min="3" max="3" width="26.6328125" customWidth="1"/>
     <col min="4" max="12" width="4.6328125" customWidth="1"/>
     <col min="13" max="13" width="8.7265625" style="14"/>
     <col min="14" max="17" width="3.36328125" customWidth="1"/>
@@ -1142,6 +1145,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="S11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -1381,6 +1387,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="S15">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -1475,7 +1484,12 @@
       <c r="J17" s="9">
         <v>5</v>
       </c>
-      <c r="L17" s="4"/>
+      <c r="K17" s="18">
+        <v>5</v>
+      </c>
+      <c r="L17" s="12">
+        <v>5</v>
+      </c>
       <c r="M17" s="16">
         <v>3</v>
       </c>
@@ -1494,6 +1508,9 @@
       <c r="Q17" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="S17">
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_21 декабря 2023 г. 13:31:08_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-422_ДисМат_.xlsx
+++ b/2ИСИП-422_ДисМат_.xlsx
@@ -600,10 +600,10 @@
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -746,6 +746,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="S4">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">

</xml_diff>